<commit_message>
edit mockups and membership management feature description
</commit_message>
<xml_diff>
--- a/ressources/project descriptions/Feature description - Membership management.xlsx
+++ b/ressources/project descriptions/Feature description - Membership management.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mathieu\Desktop\Fiches descriptives P4\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mathieu\Desktop\Projet 4 - Aller simple pour l'Alaska\project descriptions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{5A8E0850-8511-4EC6-A806-6CC9A4306AD4}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{9EAAEE63-E98F-4497-99CF-BEF0AEB6EF0D}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" tabRatio="913" firstSheet="1" activeTab="5" xr2:uid="{1B88FB64-ECA9-408D-A391-F451CFF483CD}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" tabRatio="913" activeTab="1" xr2:uid="{1B88FB64-ECA9-408D-A391-F451CFF483CD}"/>
   </bookViews>
   <sheets>
     <sheet name="FD &quot;Sign into a member account&quot;" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="548" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="550" uniqueCount="234">
   <si>
     <t>Numéro</t>
   </si>
@@ -178,9 +178,6 @@
     <t>5.1.</t>
   </si>
   <si>
-    <t>L'encart d'identification de l'utilisateur doit être positionné en haut de page et un affichage qui le met en évidence sans être trop "tape-à-l'œil" (il ne doit pas nuire à la lecture du contenu du site).</t>
-  </si>
-  <si>
     <t>Les transitions entre les différentes étapes de l'identification de l'utilisateur doit être instantané.</t>
   </si>
   <si>
@@ -193,12 +190,6 @@
     <t>Visiteur</t>
   </si>
   <si>
-    <t>Il affiche à l'utilisateur un message pour lui signaler qu'aucun compte ne correspondent aux identifiants entrés et lui propose de réessayer d'entrer ses identifiants (retour au point 4), de recevoir ses identifiants par mail (appel au cas d'utilisation "Retrieve account info") ou de créer un nouveau compte (appel du cas d'utilisation 'Create a member account').</t>
-  </si>
-  <si>
-    <t>L'utilisateur choisi une des trois options.</t>
-  </si>
-  <si>
     <t>Arrêt du cas d'utilisation.</t>
   </si>
   <si>
@@ -217,24 +208,15 @@
     <t>Il entre son adresse mail.</t>
   </si>
   <si>
-    <t>Il affiche à l'utilisateur un formulaire pour entrer son adresse mail avec un bouton 'valider' non-cliquable.</t>
-  </si>
-  <si>
     <t>Il valide le formulaire grâce au bouton 'valider'.</t>
   </si>
   <si>
-    <t>Il affiche un message à l'utilisateur pour lui informer qu'un mail lui a été envoyé, qui récapitulera les informations de connexion.</t>
-  </si>
-  <si>
     <t>Il affiche la page 'chapterList'.</t>
   </si>
   <si>
     <t>Il peut décider de ne pas entrer d'adresse mail.</t>
   </si>
   <si>
-    <t>Il peut décider de la fonctionnalité de récupération d'information de connexion.</t>
-  </si>
-  <si>
     <t>Retrieve account info (package "membership management")</t>
   </si>
   <si>
@@ -313,15 +295,6 @@
     <t>Exception E1 : au point 5, les identifiants de l'utilisateur ne correspondent à aucun utilisateur en BDD</t>
   </si>
   <si>
-    <t>Appel du cas d'utilisation dépendant de l'option choisie.</t>
-  </si>
-  <si>
-    <t>5.3</t>
-  </si>
-  <si>
-    <t>5.4.</t>
-  </si>
-  <si>
     <t>L'enregistrement d'un nouveau compte en BDD doit se faire en moins de 5 secondes.</t>
   </si>
   <si>
@@ -469,27 +442,12 @@
     <t>Il récupère en BDD le champ pseudonyme qui correspondent à l'adresse mail.</t>
   </si>
   <si>
-    <t>Il envoie un mail mis en forme avec un lien pour changer son mot de passe.</t>
-  </si>
-  <si>
     <t>Il sélectionne le lien pour changer de mot de passe.</t>
   </si>
   <si>
-    <t>Il lui affiche un formulaire pour définir un nouveau mot de passe avec un bouton 'valider' non-cliquable.</t>
-  </si>
-  <si>
-    <t>Il entre un nouveau mot de passe.</t>
-  </si>
-  <si>
     <t>12.</t>
   </si>
   <si>
-    <t>Il rend cliquable le bouton 'valider' si le champ est rempli et correspond au format d'un mail (test Regex).</t>
-  </si>
-  <si>
-    <t>Il rend cliquable le bouton 'valider' si le champ est rempli.</t>
-  </si>
-  <si>
     <t>Il envoie la requête à la BDD pour modifier le mot de passe de l'utilisateur.</t>
   </si>
   <si>
@@ -506,9 +464,6 @@
   </si>
   <si>
     <t>8.a.</t>
-  </si>
-  <si>
-    <t>8.b.</t>
   </si>
   <si>
     <t>Il peut décider de ne pas entrer de nouveau mot de passe.</t>
@@ -704,15 +659,9 @@
     <t>Il entre ses identifiants.</t>
   </si>
   <si>
-    <t>Il propose à l'utilisateur d'entrer ses identifiants et affiche un bouton 'valider' non-cliquable pour valider les données, ou de créer un nouveau compte.</t>
-  </si>
-  <si>
     <t>Il valide ses identifiants avec le bouton 'valider'.</t>
   </si>
   <si>
-    <t>Il peut décider de poursuivre sa visite sans s'enregistrer.</t>
-  </si>
-  <si>
     <t>Il rend le bouton 'valider' cliquable si tous les champs sont remplis.</t>
   </si>
   <si>
@@ -729,6 +678,66 @@
   </si>
   <si>
     <t>Il rend le bouton 'valider' cliquable si l'utilisateur remplit tous les champs, que l'adresse mail est au format 'x@y.z' (test Regex fait en quittant la saisie du mot de passe), et que les deux champs 'mot de passe' sont identiques.</t>
+  </si>
+  <si>
+    <t>Il propose à l'utilisateur d'entrer ses identifiants et affiche un bouton 'valider' non-cliquable pour se connecter avec les identifiants entrés. Il propose aussi l'option de récupérer des identifiants perdus, ou de créer un nouveau compte.</t>
+  </si>
+  <si>
+    <t>1 (version 2)</t>
+  </si>
+  <si>
+    <t>26/07/2018 (dernière version : 06/08/2018)</t>
+  </si>
+  <si>
+    <t>Il peut décider de poursuivre sa visite sans s'enregistrer en quittant la page de connexion.</t>
+  </si>
+  <si>
+    <t>Il peut décider de demander à récupérer ses identifiants (appel du cas d'utilisation 'retrieve account info'.</t>
+  </si>
+  <si>
+    <t>4.c</t>
+  </si>
+  <si>
+    <t>Il ajoute un message indiquant à l'utilisateur que les identifiants ne correspondent à aucun utilisateur.</t>
+  </si>
+  <si>
+    <t>Reprise au point 1.</t>
+  </si>
+  <si>
+    <t>L'encart d'identification de l'utilisateur doit être positionné en haut de page avec un affichage qui le met en évidence sans être trop "tape-à-l'œil" (il ne doit pas nuire à la lecture du contenu du site).</t>
+  </si>
+  <si>
+    <t>Il affiche à l'utilisateur un formulaire pour entrer son adresse mail avec un bouton 'poursuivre la procédure' non-cliquable.</t>
+  </si>
+  <si>
+    <t>Il rend le bouton 'poursuivre la procédure' cliquable si le champ est rempli et correspond au format d'un mail (test Regex).</t>
+  </si>
+  <si>
+    <t>Il valide le formulaire grâce au bouton 'poursuivre la procédure'.</t>
+  </si>
+  <si>
+    <t>Il affiche un message à l'utilisateur pour lui informer qu'un mail lui a été envoyé, qui lui permettra de définir un nouveau mot de passe.</t>
+  </si>
+  <si>
+    <t>Il envoie un mail mis en forme avec un lien pour changer le mot de passe du compte utilisateur.</t>
+  </si>
+  <si>
+    <t>Il lui affiche un formulaire avec deux champs pour définir un nouveau mot de passe avec un bouton 'valider' non-cliquable.</t>
+  </si>
+  <si>
+    <t>Il entre deux fois un même mot de passe.</t>
+  </si>
+  <si>
+    <t>Il rend cliquable le bouton 'valider' si les champs sont remplis et qu'ils sont identiques.</t>
+  </si>
+  <si>
+    <t>Il peut décider de quitter la fonctionnalité de récupération d'informations de connexion.</t>
+  </si>
+  <si>
+    <t>2 (version 2)</t>
+  </si>
+  <si>
+    <t>27/07/2018 (dernière version : 06/08/2018)</t>
   </si>
 </sst>
 </file>
@@ -1212,7 +1221,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="84">
+  <cellXfs count="85">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1401,30 +1410,30 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -1442,6 +1451,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1760,7 +1772,7 @@
   <dimension ref="A1:E52"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:C1"/>
+      <selection activeCell="B10" sqref="B10:C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1771,11 +1783,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="72" t="s">
-        <v>104</v>
-      </c>
-      <c r="B1" s="72"/>
-      <c r="C1" s="72"/>
+      <c r="A1" s="70" t="s">
+        <v>95</v>
+      </c>
+      <c r="B1" s="70"/>
+      <c r="C1" s="70"/>
     </row>
     <row r="2" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="19"/>
@@ -1787,73 +1799,73 @@
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="74">
-        <v>1</v>
-      </c>
-      <c r="C3" s="74"/>
+      <c r="B3" s="73" t="s">
+        <v>215</v>
+      </c>
+      <c r="C3" s="73"/>
     </row>
     <row r="4" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="77" t="s">
-        <v>105</v>
-      </c>
-      <c r="C4" s="77"/>
+      <c r="B4" s="74" t="s">
+        <v>96</v>
+      </c>
+      <c r="C4" s="74"/>
     </row>
     <row r="5" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B5" s="70" t="s">
+      <c r="B5" s="76" t="s">
         <v>43</v>
       </c>
-      <c r="C5" s="70"/>
+      <c r="C5" s="76"/>
     </row>
     <row r="6" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="71" t="s">
+      <c r="B6" s="75" t="s">
         <v>45</v>
       </c>
-      <c r="C6" s="71"/>
+      <c r="C6" s="75"/>
     </row>
     <row r="7" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="70" t="s">
+      <c r="B7" s="76" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="70"/>
+      <c r="C7" s="76"/>
     </row>
     <row r="8" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="76">
-        <v>43307</v>
-      </c>
-      <c r="C8" s="76"/>
+      <c r="B8" s="72" t="s">
+        <v>216</v>
+      </c>
+      <c r="C8" s="72"/>
     </row>
     <row r="9" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="70" t="s">
+      <c r="B9" s="76" t="s">
         <v>44</v>
       </c>
-      <c r="C9" s="70"/>
+      <c r="C9" s="76"/>
     </row>
     <row r="10" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="75" t="s">
-        <v>220</v>
-      </c>
-      <c r="C10" s="75"/>
+      <c r="B10" s="71" t="s">
+        <v>205</v>
+      </c>
+      <c r="C10" s="71"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="13"/>
@@ -1868,11 +1880,11 @@
       <c r="C12" s="17"/>
     </row>
     <row r="13" spans="1:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="72" t="s">
+      <c r="A13" s="70" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="72"/>
-      <c r="C13" s="72"/>
+      <c r="B13" s="70"/>
+      <c r="C13" s="70"/>
     </row>
     <row r="14" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="24"/>
@@ -1892,13 +1904,13 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
         <v>7</v>
       </c>
       <c r="B16" s="6"/>
       <c r="C16" s="6" t="s">
-        <v>222</v>
+        <v>214</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1906,7 +1918,7 @@
         <v>8</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>221</v>
+        <v>206</v>
       </c>
       <c r="C17" s="8"/>
     </row>
@@ -1916,7 +1928,7 @@
       </c>
       <c r="B18" s="6"/>
       <c r="C18" s="6" t="s">
-        <v>225</v>
+        <v>208</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1924,7 +1936,7 @@
         <v>10</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>223</v>
+        <v>207</v>
       </c>
       <c r="C19" s="8"/>
     </row>
@@ -1934,7 +1946,7 @@
       </c>
       <c r="B20" s="6"/>
       <c r="C20" s="6" t="s">
-        <v>226</v>
+        <v>209</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1943,7 +1955,7 @@
       </c>
       <c r="B21" s="10"/>
       <c r="C21" s="8" t="s">
-        <v>227</v>
+        <v>210</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1952,7 +1964,7 @@
       </c>
       <c r="B22" s="6"/>
       <c r="C22" s="6" t="s">
-        <v>228</v>
+        <v>211</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -1963,11 +1975,11 @@
       <c r="C24" s="31"/>
     </row>
     <row r="25" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="72" t="s">
+      <c r="A25" s="70" t="s">
         <v>19</v>
       </c>
-      <c r="B25" s="72"/>
-      <c r="C25" s="72"/>
+      <c r="B25" s="70"/>
+      <c r="C25" s="70"/>
     </row>
     <row r="26" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="38"/>
@@ -1987,107 +1999,107 @@
     </row>
     <row r="28" spans="1:4" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="5" t="s">
-        <v>17</v>
+        <v>42</v>
       </c>
       <c r="B28" s="6" t="s">
         <v>46</v>
       </c>
       <c r="C28" s="6"/>
     </row>
-    <row r="29" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="7" t="s">
+    <row r="29" spans="1:4" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="B29" s="39" t="s">
-        <v>224</v>
-      </c>
-      <c r="C29" s="9"/>
-    </row>
-    <row r="30" spans="1:4" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B29" s="10" t="s">
+        <v>218</v>
+      </c>
+      <c r="C29" s="10"/>
+    </row>
+    <row r="30" spans="1:4" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="B30" s="6" t="s">
+        <v>179</v>
+      </c>
+      <c r="B30" s="68" t="s">
+        <v>217</v>
+      </c>
+      <c r="C30" s="6"/>
+    </row>
+    <row r="31" spans="1:4" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="B31" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="C30" s="6"/>
-    </row>
-    <row r="31" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="B31" s="39" t="s">
-        <v>224</v>
-      </c>
-      <c r="C31" s="9"/>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="15"/>
-      <c r="B32" s="15"/>
-      <c r="C32" s="15"/>
-    </row>
-    <row r="33" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="21"/>
-      <c r="B33" s="21"/>
-      <c r="C33" s="22"/>
-    </row>
-    <row r="34" spans="1:4" ht="38.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="73" t="s">
-        <v>92</v>
-      </c>
-      <c r="B34" s="73"/>
-      <c r="C34" s="73"/>
+      <c r="C31" s="10"/>
+    </row>
+    <row r="32" spans="1:4" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B32" s="6" t="s">
+        <v>218</v>
+      </c>
+      <c r="C32" s="6"/>
+    </row>
+    <row r="33" spans="1:4" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="7" t="s">
+        <v>219</v>
+      </c>
+      <c r="B33" s="84" t="s">
+        <v>217</v>
+      </c>
+      <c r="C33" s="9"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="15"/>
+      <c r="B34" s="15"/>
+      <c r="C34" s="15"/>
     </row>
     <row r="35" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="27"/>
-      <c r="B35" s="28"/>
-      <c r="C35" s="25"/>
-    </row>
-    <row r="36" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="3" t="s">
+      <c r="A35" s="21"/>
+      <c r="B35" s="21"/>
+      <c r="C35" s="22"/>
+    </row>
+    <row r="36" spans="1:4" ht="38.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="77" t="s">
+        <v>86</v>
+      </c>
+      <c r="B36" s="77"/>
+      <c r="C36" s="77"/>
+    </row>
+    <row r="37" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="27"/>
+      <c r="B37" s="28"/>
+      <c r="C37" s="25"/>
+    </row>
+    <row r="38" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B36" s="4" t="s">
+      <c r="B38" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C36" s="4" t="s">
+      <c r="C38" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="5" t="s">
+    <row r="39" spans="1:4" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="5" t="s">
         <v>47</v>
-      </c>
-      <c r="B37" s="6"/>
-      <c r="C37" s="6" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="B38" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="C38" s="10"/>
-    </row>
-    <row r="39" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="5" t="s">
-        <v>94</v>
       </c>
       <c r="B39" s="6"/>
       <c r="C39" s="6" t="s">
-        <v>93</v>
+        <v>220</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="41" t="s">
-        <v>95</v>
-      </c>
-      <c r="B40" s="9"/>
-      <c r="C40" s="9" t="s">
-        <v>55</v>
+      <c r="A40" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B40" s="10"/>
+      <c r="C40" s="10" t="s">
+        <v>221</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -2105,19 +2117,19 @@
       <c r="A43" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B43" s="74" t="s">
-        <v>56</v>
-      </c>
-      <c r="C43" s="74"/>
+      <c r="B43" s="73" t="s">
+        <v>53</v>
+      </c>
+      <c r="C43" s="73"/>
     </row>
     <row r="44" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B44" s="71" t="s">
+      <c r="B44" s="75" t="s">
         <v>36</v>
       </c>
-      <c r="C44" s="71"/>
+      <c r="C44" s="75"/>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="63"/>
@@ -2131,11 +2143,11 @@
       <c r="D46" s="31"/>
     </row>
     <row r="47" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="72" t="s">
+      <c r="A47" s="70" t="s">
         <v>23</v>
       </c>
-      <c r="B47" s="72"/>
-      <c r="C47" s="72"/>
+      <c r="B47" s="70"/>
+      <c r="C47" s="70"/>
     </row>
     <row r="48" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="30"/>
@@ -2146,28 +2158,28 @@
       <c r="A49" s="54" t="s">
         <v>24</v>
       </c>
-      <c r="B49" s="70" t="s">
-        <v>48</v>
-      </c>
-      <c r="C49" s="70"/>
+      <c r="B49" s="76" t="s">
+        <v>222</v>
+      </c>
+      <c r="C49" s="76"/>
     </row>
     <row r="50" spans="1:3" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="55" t="s">
         <v>25</v>
       </c>
-      <c r="B50" s="71" t="s">
-        <v>49</v>
-      </c>
-      <c r="C50" s="71"/>
+      <c r="B50" s="75" t="s">
+        <v>48</v>
+      </c>
+      <c r="C50" s="75"/>
     </row>
     <row r="51" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="66" t="s">
         <v>26</v>
       </c>
-      <c r="B51" s="70" t="s">
-        <v>50</v>
-      </c>
-      <c r="C51" s="70"/>
+      <c r="B51" s="76" t="s">
+        <v>49</v>
+      </c>
+      <c r="C51" s="76"/>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="31"/>
@@ -2175,6 +2187,15 @@
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="18">
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="A13:C13"/>
+    <mergeCell ref="A47:C47"/>
+    <mergeCell ref="A36:C36"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="A25:C25"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="B10:C10"/>
     <mergeCell ref="B8:C8"/>
@@ -2184,15 +2205,6 @@
     <mergeCell ref="B9:C9"/>
     <mergeCell ref="B5:C5"/>
     <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="B50:C50"/>
-    <mergeCell ref="B51:C51"/>
-    <mergeCell ref="A13:C13"/>
-    <mergeCell ref="A47:C47"/>
-    <mergeCell ref="A34:C34"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="A25:C25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2201,9 +2213,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABDD6380-E7EE-435B-8D4A-B8FA31D1FD4A}">
-  <dimension ref="A1:D65"/>
+  <dimension ref="A1:D64"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
@@ -2216,7 +2228,7 @@
   <sheetData>
     <row r="1" spans="1:3" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="78" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B1" s="79"/>
       <c r="C1" s="80"/>
@@ -2230,73 +2242,73 @@
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="74">
-        <v>2</v>
-      </c>
-      <c r="C3" s="74"/>
+      <c r="B3" s="73" t="s">
+        <v>232</v>
+      </c>
+      <c r="C3" s="73"/>
     </row>
     <row r="4" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="77" t="s">
-        <v>67</v>
-      </c>
-      <c r="C4" s="77"/>
+      <c r="B4" s="74" t="s">
+        <v>61</v>
+      </c>
+      <c r="C4" s="74"/>
     </row>
     <row r="5" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B5" s="70" t="s">
-        <v>52</v>
-      </c>
-      <c r="C5" s="70"/>
+      <c r="B5" s="76" t="s">
+        <v>51</v>
+      </c>
+      <c r="C5" s="76"/>
     </row>
     <row r="6" spans="1:3" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="71" t="s">
-        <v>58</v>
-      </c>
-      <c r="C6" s="71"/>
+      <c r="B6" s="75" t="s">
+        <v>55</v>
+      </c>
+      <c r="C6" s="75"/>
     </row>
     <row r="7" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="70" t="s">
+      <c r="B7" s="76" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="70"/>
+      <c r="C7" s="76"/>
     </row>
     <row r="8" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="76">
-        <v>43308</v>
-      </c>
-      <c r="C8" s="76"/>
+      <c r="B8" s="72" t="s">
+        <v>233</v>
+      </c>
+      <c r="C8" s="72"/>
     </row>
     <row r="9" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="70" t="s">
+      <c r="B9" s="76" t="s">
         <v>44</v>
       </c>
-      <c r="C9" s="70"/>
+      <c r="C9" s="76"/>
     </row>
     <row r="10" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="75" t="s">
-        <v>59</v>
-      </c>
-      <c r="C10" s="75"/>
+      <c r="B10" s="71" t="s">
+        <v>56</v>
+      </c>
+      <c r="C10" s="71"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="36"/>
@@ -2309,11 +2321,11 @@
       <c r="C12" s="28"/>
     </row>
     <row r="13" spans="1:3" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="72" t="s">
+      <c r="A13" s="70" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="72"/>
-      <c r="C13" s="72"/>
+      <c r="B13" s="70"/>
+      <c r="C13" s="70"/>
     </row>
     <row r="14" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="38"/>
@@ -2331,13 +2343,13 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
         <v>7</v>
       </c>
       <c r="B16" s="6"/>
       <c r="C16" s="6" t="s">
-        <v>61</v>
+        <v>223</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2345,25 +2357,25 @@
         <v>8</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C17" s="8"/>
     </row>
-    <row r="18" spans="1:3" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
         <v>9</v>
       </c>
       <c r="B18" s="6"/>
       <c r="C18" s="6" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="41" t="s">
         <v>10</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>62</v>
+        <v>225</v>
       </c>
       <c r="C19" s="9"/>
     </row>
@@ -2373,7 +2385,7 @@
       </c>
       <c r="B20" s="6"/>
       <c r="C20" s="6" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2382,7 +2394,7 @@
       </c>
       <c r="B21" s="9"/>
       <c r="C21" s="9" t="s">
-        <v>63</v>
+        <v>226</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2391,7 +2403,7 @@
       </c>
       <c r="B22" s="6"/>
       <c r="C22" s="6" t="s">
-        <v>145</v>
+        <v>227</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2399,80 +2411,80 @@
         <v>34</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>146</v>
+        <v>136</v>
       </c>
       <c r="C23" s="9"/>
     </row>
-    <row r="24" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
         <v>35</v>
       </c>
       <c r="B24" s="6"/>
       <c r="C24" s="6" t="s">
-        <v>147</v>
+        <v>228</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="41" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>148</v>
+        <v>229</v>
       </c>
       <c r="C25" s="9"/>
     </row>
     <row r="26" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="5" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="B26" s="6"/>
       <c r="C26" s="6" t="s">
-        <v>151</v>
+        <v>230</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="41" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C27" s="9"/>
     </row>
     <row r="28" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="5" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="B28" s="6"/>
       <c r="C28" s="6" t="s">
-        <v>152</v>
+        <v>138</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="41" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="B29" s="9"/>
       <c r="C29" s="9" t="s">
-        <v>153</v>
+        <v>139</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="5" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="B30" s="6"/>
       <c r="C30" s="6" t="s">
-        <v>154</v>
+        <v>140</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="41" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="B31" s="9"/>
       <c r="C31" s="9" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
@@ -2486,11 +2498,11 @@
       <c r="C33" s="31"/>
     </row>
     <row r="34" spans="1:3" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="72" t="s">
+      <c r="A34" s="70" t="s">
         <v>19</v>
       </c>
-      <c r="B34" s="72"/>
-      <c r="C34" s="72"/>
+      <c r="B34" s="70"/>
+      <c r="C34" s="70"/>
     </row>
     <row r="35" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="38"/>
@@ -2513,7 +2525,7 @@
         <v>42</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="C37" s="6"/>
     </row>
@@ -2522,237 +2534,228 @@
         <v>20</v>
       </c>
       <c r="B38" s="39" t="s">
-        <v>66</v>
+        <v>231</v>
       </c>
       <c r="C38" s="9"/>
     </row>
     <row r="39" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="5" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="C39" s="6"/>
     </row>
     <row r="40" spans="1:3" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="7" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="B40" s="39" t="s">
-        <v>156</v>
+        <v>231</v>
       </c>
       <c r="C40" s="9"/>
     </row>
     <row r="41" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="5" t="s">
-        <v>157</v>
+        <v>143</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>155</v>
+        <v>141</v>
       </c>
       <c r="C41" s="6"/>
     </row>
     <row r="42" spans="1:3" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="7" t="s">
-        <v>158</v>
-      </c>
-      <c r="B42" s="39" t="s">
-        <v>156</v>
-      </c>
-      <c r="C42" s="9"/>
+      <c r="A42" s="12" t="s">
+        <v>145</v>
+      </c>
+      <c r="B42" s="10" t="s">
+        <v>144</v>
+      </c>
+      <c r="C42" s="10"/>
     </row>
     <row r="43" spans="1:3" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="5" t="s">
-        <v>160</v>
-      </c>
-      <c r="B43" s="6" t="s">
-        <v>159</v>
+        <v>146</v>
+      </c>
+      <c r="B43" s="68" t="s">
+        <v>142</v>
       </c>
       <c r="C43" s="6"/>
     </row>
     <row r="44" spans="1:3" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="7" t="s">
-        <v>161</v>
-      </c>
-      <c r="B44" s="39" t="s">
-        <v>156</v>
-      </c>
-      <c r="C44" s="9"/>
+      <c r="A44" s="12" t="s">
+        <v>147</v>
+      </c>
+      <c r="B44" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="C44" s="10"/>
     </row>
     <row r="45" spans="1:3" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="5" t="s">
-        <v>162</v>
-      </c>
-      <c r="B45" s="6" t="s">
-        <v>164</v>
+        <v>148</v>
+      </c>
+      <c r="B45" s="68" t="s">
+        <v>142</v>
       </c>
       <c r="C45" s="6"/>
     </row>
-    <row r="46" spans="1:3" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="7" t="s">
-        <v>163</v>
-      </c>
-      <c r="B46" s="39" t="s">
-        <v>156</v>
-      </c>
-      <c r="C46" s="9"/>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" s="15"/>
-      <c r="B47" s="15"/>
-      <c r="C47" s="15"/>
-    </row>
-    <row r="48" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="31"/>
-      <c r="B48" s="31"/>
-      <c r="C48" s="31"/>
-    </row>
-    <row r="49" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="72" t="s">
-        <v>91</v>
-      </c>
-      <c r="B49" s="72"/>
-      <c r="C49" s="72"/>
-    </row>
-    <row r="50" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="38"/>
-      <c r="B50" s="37"/>
-      <c r="C50" s="37"/>
-    </row>
-    <row r="51" spans="1:4" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="3" t="s">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" s="15"/>
+      <c r="B46" s="15"/>
+      <c r="C46" s="15"/>
+    </row>
+    <row r="47" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="31"/>
+      <c r="B47" s="31"/>
+      <c r="C47" s="31"/>
+    </row>
+    <row r="48" spans="1:3" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="70" t="s">
+        <v>85</v>
+      </c>
+      <c r="B48" s="70"/>
+      <c r="C48" s="70"/>
+    </row>
+    <row r="49" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="38"/>
+      <c r="B49" s="37"/>
+      <c r="C49" s="37"/>
+    </row>
+    <row r="50" spans="1:4" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B51" s="4" t="s">
+      <c r="B50" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C51" s="4" t="s">
+      <c r="C50" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="52" spans="1:4" ht="46.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="B52" s="6"/>
-      <c r="C52" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="D52" s="31"/>
-    </row>
-    <row r="53" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="41" t="s">
+    <row r="51" spans="1:4" ht="46.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B51" s="6"/>
+      <c r="C51" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="D51" s="31"/>
+    </row>
+    <row r="52" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="41" t="s">
         <v>28</v>
       </c>
-      <c r="B53" s="9"/>
-      <c r="C53" s="9" t="s">
+      <c r="B52" s="9"/>
+      <c r="C52" s="9" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" s="31"/>
+      <c r="B53" s="1"/>
+      <c r="C53" s="43"/>
+    </row>
+    <row r="54" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="31"/>
-      <c r="B54" s="1"/>
-      <c r="C54" s="43"/>
+      <c r="B54" s="31"/>
+      <c r="C54" s="31"/>
     </row>
     <row r="55" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="31"/>
-      <c r="B55" s="31"/>
-      <c r="C55" s="31"/>
+      <c r="A55" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B55" s="73" t="s">
+        <v>150</v>
+      </c>
+      <c r="C55" s="73"/>
     </row>
     <row r="56" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B56" s="74" t="s">
-        <v>165</v>
-      </c>
-      <c r="C56" s="74"/>
-    </row>
-    <row r="57" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="3" t="s">
+      <c r="A56" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B57" s="71" t="s">
-        <v>166</v>
-      </c>
-      <c r="C57" s="71"/>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" s="15"/>
-      <c r="B58" s="15"/>
-      <c r="C58" s="15"/>
-    </row>
-    <row r="59" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="31"/>
-      <c r="B59" s="1"/>
-      <c r="C59" s="43"/>
+      <c r="B56" s="75" t="s">
+        <v>151</v>
+      </c>
+      <c r="C56" s="75"/>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" s="15"/>
+      <c r="B57" s="15"/>
+      <c r="C57" s="15"/>
+    </row>
+    <row r="58" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A58" s="31"/>
+      <c r="B58" s="1"/>
+      <c r="C58" s="43"/>
+    </row>
+    <row r="59" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="70" t="s">
+        <v>23</v>
+      </c>
+      <c r="B59" s="70"/>
+      <c r="C59" s="70"/>
     </row>
     <row r="60" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="72" t="s">
-        <v>23</v>
-      </c>
-      <c r="B60" s="72"/>
-      <c r="C60" s="72"/>
-    </row>
-    <row r="61" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="40"/>
-      <c r="B61" s="40"/>
-      <c r="C61" s="40"/>
-    </row>
-    <row r="62" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="2" t="s">
+      <c r="A60" s="40"/>
+      <c r="B60" s="40"/>
+      <c r="C60" s="40"/>
+    </row>
+    <row r="61" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A61" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B62" s="70" t="s">
-        <v>50</v>
-      </c>
-      <c r="C62" s="70"/>
-    </row>
-    <row r="63" spans="1:4" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="3" t="s">
+      <c r="B61" s="76" t="s">
+        <v>49</v>
+      </c>
+      <c r="C61" s="76"/>
+    </row>
+    <row r="62" spans="1:4" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A62" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B63" s="71" t="s">
-        <v>72</v>
-      </c>
-      <c r="C63" s="71"/>
-    </row>
-    <row r="64" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="2" t="s">
+      <c r="B62" s="75" t="s">
+        <v>66</v>
+      </c>
+      <c r="C62" s="75"/>
+    </row>
+    <row r="63" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A63" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B64" s="70" t="s">
-        <v>50</v>
-      </c>
-      <c r="C64" s="70"/>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A65" s="32"/>
-      <c r="B65" s="33"/>
-      <c r="C65" s="34"/>
+      <c r="B63" s="76" t="s">
+        <v>49</v>
+      </c>
+      <c r="C63" s="76"/>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64" s="32"/>
+      <c r="B64" s="33"/>
+      <c r="C64" s="34"/>
     </row>
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="18">
+    <mergeCell ref="B63:C63"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="A13:C13"/>
+    <mergeCell ref="A34:C34"/>
+    <mergeCell ref="A48:C48"/>
+    <mergeCell ref="B55:C55"/>
+    <mergeCell ref="B56:C56"/>
+    <mergeCell ref="A59:C59"/>
+    <mergeCell ref="B61:C61"/>
+    <mergeCell ref="B62:C62"/>
     <mergeCell ref="B7:C7"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="B5:C5"/>
     <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B64:C64"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="A13:C13"/>
-    <mergeCell ref="A34:C34"/>
-    <mergeCell ref="A49:C49"/>
-    <mergeCell ref="B56:C56"/>
-    <mergeCell ref="B57:C57"/>
-    <mergeCell ref="A60:C60"/>
-    <mergeCell ref="B62:C62"/>
-    <mergeCell ref="B63:C63"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
@@ -2776,7 +2779,7 @@
   <sheetData>
     <row r="1" spans="1:3" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="78" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B1" s="79"/>
       <c r="C1" s="80"/>
@@ -2790,73 +2793,73 @@
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="74">
+      <c r="B3" s="73">
         <v>3</v>
       </c>
-      <c r="C3" s="74"/>
+      <c r="C3" s="73"/>
     </row>
     <row r="4" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="77" t="s">
-        <v>73</v>
-      </c>
-      <c r="C4" s="77"/>
+      <c r="B4" s="74" t="s">
+        <v>67</v>
+      </c>
+      <c r="C4" s="74"/>
     </row>
     <row r="5" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B5" s="70" t="s">
-        <v>52</v>
-      </c>
-      <c r="C5" s="70"/>
+      <c r="B5" s="76" t="s">
+        <v>51</v>
+      </c>
+      <c r="C5" s="76"/>
     </row>
     <row r="6" spans="1:3" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="71" t="s">
-        <v>74</v>
-      </c>
-      <c r="C6" s="71"/>
+      <c r="B6" s="75" t="s">
+        <v>68</v>
+      </c>
+      <c r="C6" s="75"/>
     </row>
     <row r="7" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="70" t="s">
+      <c r="B7" s="76" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="70"/>
+      <c r="C7" s="76"/>
     </row>
     <row r="8" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="76">
+      <c r="B8" s="72">
         <v>43308</v>
       </c>
-      <c r="C8" s="76"/>
+      <c r="C8" s="72"/>
     </row>
     <row r="9" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="70" t="s">
-        <v>99</v>
-      </c>
-      <c r="C9" s="70"/>
+      <c r="B9" s="76" t="s">
+        <v>90</v>
+      </c>
+      <c r="C9" s="76"/>
     </row>
     <row r="10" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="75" t="s">
-        <v>103</v>
-      </c>
-      <c r="C10" s="75"/>
+      <c r="B10" s="71" t="s">
+        <v>94</v>
+      </c>
+      <c r="C10" s="71"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="36"/>
@@ -2869,11 +2872,11 @@
       <c r="C12" s="28"/>
     </row>
     <row r="13" spans="1:3" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="72" t="s">
+      <c r="A13" s="70" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="72"/>
-      <c r="C13" s="72"/>
+      <c r="B13" s="70"/>
+      <c r="C13" s="70"/>
     </row>
     <row r="14" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="38"/>
@@ -2897,7 +2900,7 @@
       </c>
       <c r="B16" s="6"/>
       <c r="C16" s="6" t="s">
-        <v>229</v>
+        <v>212</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2905,7 +2908,7 @@
         <v>8</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="C17" s="8"/>
     </row>
@@ -2915,7 +2918,7 @@
       </c>
       <c r="B18" s="6"/>
       <c r="C18" s="6" t="s">
-        <v>230</v>
+        <v>213</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2923,7 +2926,7 @@
         <v>10</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="C19" s="9"/>
     </row>
@@ -2933,7 +2936,7 @@
       </c>
       <c r="B20" s="6"/>
       <c r="C20" s="6" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2942,7 +2945,7 @@
       </c>
       <c r="B21" s="9"/>
       <c r="C21" s="9" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2951,7 +2954,7 @@
       </c>
       <c r="B22" s="6"/>
       <c r="C22" s="6" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -2965,11 +2968,11 @@
       <c r="C24" s="31"/>
     </row>
     <row r="25" spans="1:3" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="72" t="s">
+      <c r="A25" s="70" t="s">
         <v>19</v>
       </c>
-      <c r="B25" s="72"/>
-      <c r="C25" s="72"/>
+      <c r="B25" s="70"/>
+      <c r="C25" s="70"/>
     </row>
     <row r="26" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="38"/>
@@ -2992,7 +2995,7 @@
         <v>42</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="C28" s="6"/>
     </row>
@@ -3001,25 +3004,25 @@
         <v>20</v>
       </c>
       <c r="B29" s="67" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="C29" s="9"/>
     </row>
     <row r="30" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="5" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="C30" s="6"/>
     </row>
     <row r="31" spans="1:3" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="41" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="B31" s="67" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="C31" s="9"/>
     </row>
@@ -3034,11 +3037,11 @@
       <c r="C33" s="31"/>
     </row>
     <row r="34" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="72" t="s">
-        <v>85</v>
-      </c>
-      <c r="B34" s="72"/>
-      <c r="C34" s="72"/>
+      <c r="A34" s="70" t="s">
+        <v>79</v>
+      </c>
+      <c r="B34" s="70"/>
+      <c r="C34" s="70"/>
     </row>
     <row r="35" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="38"/>
@@ -3058,11 +3061,11 @@
     </row>
     <row r="37" spans="1:4" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="5" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="B37" s="6"/>
       <c r="C37" s="6" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="D37" s="31"/>
     </row>
@@ -3087,7 +3090,7 @@
     </row>
     <row r="41" spans="1:4" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="81" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="B41" s="82"/>
       <c r="C41" s="83"/>
@@ -3124,7 +3127,7 @@
       </c>
       <c r="B45" s="9"/>
       <c r="C45" s="9" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="D45" s="31"/>
     </row>
@@ -3148,11 +3151,11 @@
       <c r="C48" s="31"/>
     </row>
     <row r="49" spans="1:4" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="73" t="s">
-        <v>88</v>
-      </c>
-      <c r="B49" s="73"/>
-      <c r="C49" s="73"/>
+      <c r="A49" s="77" t="s">
+        <v>82</v>
+      </c>
+      <c r="B49" s="77"/>
+      <c r="C49" s="77"/>
     </row>
     <row r="50" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="38"/>
@@ -3176,7 +3179,7 @@
       </c>
       <c r="B52" s="6"/>
       <c r="C52" s="6" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="D52" s="31"/>
     </row>
@@ -3203,19 +3206,19 @@
       <c r="A56" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B56" s="74" t="s">
+      <c r="B56" s="73" t="s">
         <v>39</v>
       </c>
-      <c r="C56" s="74"/>
+      <c r="C56" s="73"/>
     </row>
     <row r="57" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B57" s="71" t="s">
-        <v>86</v>
-      </c>
-      <c r="C57" s="71"/>
+      <c r="B57" s="75" t="s">
+        <v>80</v>
+      </c>
+      <c r="C57" s="75"/>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="15"/>
@@ -3228,11 +3231,11 @@
       <c r="C59" s="43"/>
     </row>
     <row r="60" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="72" t="s">
+      <c r="A60" s="70" t="s">
         <v>23</v>
       </c>
-      <c r="B60" s="72"/>
-      <c r="C60" s="72"/>
+      <c r="B60" s="70"/>
+      <c r="C60" s="70"/>
     </row>
     <row r="61" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A61" s="40"/>
@@ -3243,28 +3246,28 @@
       <c r="A62" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B62" s="70" t="s">
-        <v>50</v>
-      </c>
-      <c r="C62" s="70"/>
+      <c r="B62" s="76" t="s">
+        <v>49</v>
+      </c>
+      <c r="C62" s="76"/>
     </row>
     <row r="63" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A63" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B63" s="71" t="s">
-        <v>96</v>
-      </c>
-      <c r="C63" s="71"/>
+      <c r="B63" s="75" t="s">
+        <v>87</v>
+      </c>
+      <c r="C63" s="75"/>
     </row>
     <row r="64" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A64" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B64" s="70" t="s">
-        <v>50</v>
-      </c>
-      <c r="C64" s="70"/>
+      <c r="B64" s="76" t="s">
+        <v>49</v>
+      </c>
+      <c r="C64" s="76"/>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" s="32"/>
@@ -3274,6 +3277,11 @@
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="20">
+    <mergeCell ref="B57:C57"/>
+    <mergeCell ref="A60:C60"/>
+    <mergeCell ref="B62:C62"/>
+    <mergeCell ref="B63:C63"/>
+    <mergeCell ref="B64:C64"/>
     <mergeCell ref="A34:C34"/>
     <mergeCell ref="B56:C56"/>
     <mergeCell ref="A1:C1"/>
@@ -3289,11 +3297,6 @@
     <mergeCell ref="A25:C25"/>
     <mergeCell ref="A49:C49"/>
     <mergeCell ref="A41:C41"/>
-    <mergeCell ref="B57:C57"/>
-    <mergeCell ref="A60:C60"/>
-    <mergeCell ref="B62:C62"/>
-    <mergeCell ref="B63:C63"/>
-    <mergeCell ref="B64:C64"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3305,7 +3308,7 @@
   <dimension ref="A1:C29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C1"/>
+      <selection activeCell="B6" sqref="B6:C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3317,7 +3320,7 @@
   <sheetData>
     <row r="1" spans="1:3" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="78" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="B1" s="79"/>
       <c r="C1" s="80"/>
@@ -3331,73 +3334,73 @@
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="74">
+      <c r="B3" s="73">
         <v>4</v>
       </c>
-      <c r="C3" s="74"/>
+      <c r="C3" s="73"/>
     </row>
     <row r="4" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="77" t="s">
-        <v>102</v>
-      </c>
-      <c r="C4" s="77"/>
+      <c r="B4" s="74" t="s">
+        <v>93</v>
+      </c>
+      <c r="C4" s="74"/>
     </row>
     <row r="5" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B5" s="70" t="s">
-        <v>97</v>
-      </c>
-      <c r="C5" s="70"/>
+      <c r="B5" s="76" t="s">
+        <v>88</v>
+      </c>
+      <c r="C5" s="76"/>
     </row>
     <row r="6" spans="1:3" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="71" t="s">
-        <v>98</v>
-      </c>
-      <c r="C6" s="71"/>
+      <c r="B6" s="75" t="s">
+        <v>89</v>
+      </c>
+      <c r="C6" s="75"/>
     </row>
     <row r="7" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="70" t="s">
+      <c r="B7" s="76" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="70"/>
+      <c r="C7" s="76"/>
     </row>
     <row r="8" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="76">
+      <c r="B8" s="72">
         <v>43308</v>
       </c>
-      <c r="C8" s="76"/>
+      <c r="C8" s="72"/>
     </row>
     <row r="9" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="70" t="s">
-        <v>100</v>
-      </c>
-      <c r="C9" s="70"/>
+      <c r="B9" s="76" t="s">
+        <v>91</v>
+      </c>
+      <c r="C9" s="76"/>
     </row>
     <row r="10" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="75" t="s">
-        <v>106</v>
-      </c>
-      <c r="C10" s="75"/>
+      <c r="B10" s="71" t="s">
+        <v>97</v>
+      </c>
+      <c r="C10" s="71"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="36"/>
@@ -3410,11 +3413,11 @@
       <c r="C12" s="28"/>
     </row>
     <row r="13" spans="1:3" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="72" t="s">
+      <c r="A13" s="70" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="72"/>
-      <c r="C13" s="72"/>
+      <c r="B13" s="70"/>
+      <c r="C13" s="70"/>
     </row>
     <row r="14" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="38"/>
@@ -3438,7 +3441,7 @@
       </c>
       <c r="B16" s="6"/>
       <c r="C16" s="6" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3447,7 +3450,7 @@
       </c>
       <c r="B17" s="8"/>
       <c r="C17" s="8" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -3464,19 +3467,19 @@
       <c r="A20" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B20" s="74" t="s">
+      <c r="B20" s="73" t="s">
         <v>36</v>
       </c>
-      <c r="C20" s="74"/>
+      <c r="C20" s="73"/>
     </row>
     <row r="21" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B21" s="71" t="s">
+      <c r="B21" s="75" t="s">
         <v>36</v>
       </c>
-      <c r="C21" s="71"/>
+      <c r="C21" s="75"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="15"/>
@@ -3489,11 +3492,11 @@
       <c r="C23" s="43"/>
     </row>
     <row r="24" spans="1:3" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="72" t="s">
+      <c r="A24" s="70" t="s">
         <v>23</v>
       </c>
-      <c r="B24" s="72"/>
-      <c r="C24" s="72"/>
+      <c r="B24" s="70"/>
+      <c r="C24" s="70"/>
     </row>
     <row r="25" spans="1:3" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="40"/>
@@ -3504,28 +3507,28 @@
       <c r="A26" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B26" s="70" t="s">
+      <c r="B26" s="76" t="s">
         <v>33</v>
       </c>
-      <c r="C26" s="70"/>
+      <c r="C26" s="76"/>
     </row>
     <row r="27" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B27" s="71" t="s">
+      <c r="B27" s="75" t="s">
         <v>36</v>
       </c>
-      <c r="C27" s="71"/>
+      <c r="C27" s="75"/>
     </row>
     <row r="28" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B28" s="70" t="s">
-        <v>50</v>
-      </c>
-      <c r="C28" s="70"/>
+      <c r="B28" s="76" t="s">
+        <v>49</v>
+      </c>
+      <c r="C28" s="76"/>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="32"/>
@@ -3535,12 +3538,6 @@
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="16">
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B6:C6"/>
     <mergeCell ref="B28:C28"/>
     <mergeCell ref="B8:C8"/>
     <mergeCell ref="B9:C9"/>
@@ -3551,6 +3548,12 @@
     <mergeCell ref="A24:C24"/>
     <mergeCell ref="B26:C26"/>
     <mergeCell ref="B27:C27"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B6:C6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3573,7 +3576,7 @@
   <sheetData>
     <row r="1" spans="1:3" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="78" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="B1" s="79"/>
       <c r="C1" s="80"/>
@@ -3587,73 +3590,73 @@
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="74">
+      <c r="B3" s="73">
         <v>5</v>
       </c>
-      <c r="C3" s="74"/>
+      <c r="C3" s="73"/>
     </row>
     <row r="4" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="77" t="s">
-        <v>111</v>
-      </c>
-      <c r="C4" s="77"/>
+      <c r="B4" s="74" t="s">
+        <v>102</v>
+      </c>
+      <c r="C4" s="74"/>
     </row>
     <row r="5" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B5" s="70" t="s">
-        <v>97</v>
-      </c>
-      <c r="C5" s="70"/>
+      <c r="B5" s="76" t="s">
+        <v>88</v>
+      </c>
+      <c r="C5" s="76"/>
     </row>
     <row r="6" spans="1:3" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="71" t="s">
-        <v>182</v>
-      </c>
-      <c r="C6" s="71"/>
+      <c r="B6" s="75" t="s">
+        <v>167</v>
+      </c>
+      <c r="C6" s="75"/>
     </row>
     <row r="7" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="70" t="s">
+      <c r="B7" s="76" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="70"/>
+      <c r="C7" s="76"/>
     </row>
     <row r="8" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="76">
+      <c r="B8" s="72">
         <v>43309</v>
       </c>
-      <c r="C8" s="76"/>
+      <c r="C8" s="72"/>
     </row>
     <row r="9" spans="1:3" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="70" t="s">
-        <v>183</v>
-      </c>
-      <c r="C9" s="70"/>
+      <c r="B9" s="76" t="s">
+        <v>168</v>
+      </c>
+      <c r="C9" s="76"/>
     </row>
     <row r="10" spans="1:3" ht="62.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="75" t="s">
-        <v>188</v>
-      </c>
-      <c r="C10" s="75"/>
+      <c r="B10" s="71" t="s">
+        <v>173</v>
+      </c>
+      <c r="C10" s="71"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="36"/>
@@ -3666,11 +3669,11 @@
       <c r="C12" s="28"/>
     </row>
     <row r="13" spans="1:3" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="72" t="s">
+      <c r="A13" s="70" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="72"/>
-      <c r="C13" s="72"/>
+      <c r="B13" s="70"/>
+      <c r="C13" s="70"/>
     </row>
     <row r="14" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="38"/>
@@ -3694,7 +3697,7 @@
       </c>
       <c r="B16" s="6"/>
       <c r="C16" s="6" t="s">
-        <v>187</v>
+        <v>172</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3702,7 +3705,7 @@
         <v>8</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="C17" s="8"/>
     </row>
@@ -3712,7 +3715,7 @@
       </c>
       <c r="B18" s="6"/>
       <c r="C18" s="6" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3720,7 +3723,7 @@
         <v>10</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="C19" s="9"/>
     </row>
@@ -3730,7 +3733,7 @@
       </c>
       <c r="B20" s="6"/>
       <c r="C20" s="6" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3739,7 +3742,7 @@
       </c>
       <c r="B21" s="9"/>
       <c r="C21" s="9" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3748,7 +3751,7 @@
       </c>
       <c r="B22" s="6"/>
       <c r="C22" s="6" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
@@ -3762,11 +3765,11 @@
       <c r="C24" s="31"/>
     </row>
     <row r="25" spans="1:7" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="72" t="s">
+      <c r="A25" s="70" t="s">
         <v>19</v>
       </c>
-      <c r="B25" s="72"/>
-      <c r="C25" s="72"/>
+      <c r="B25" s="70"/>
+      <c r="C25" s="70"/>
     </row>
     <row r="26" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="38"/>
@@ -3789,7 +3792,7 @@
         <v>42</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
       <c r="C28" s="6"/>
     </row>
@@ -3798,25 +3801,25 @@
         <v>20</v>
       </c>
       <c r="B29" s="67" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="C29" s="9"/>
     </row>
     <row r="30" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="5" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="C30" s="6"/>
     </row>
     <row r="31" spans="1:7" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="41" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="B31" s="67" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="C31" s="9"/>
       <c r="G31" s="31"/>
@@ -3832,11 +3835,11 @@
       <c r="C33" s="15"/>
     </row>
     <row r="34" spans="1:3" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="72" t="s">
-        <v>120</v>
-      </c>
-      <c r="B34" s="72"/>
-      <c r="C34" s="72"/>
+      <c r="A34" s="70" t="s">
+        <v>111</v>
+      </c>
+      <c r="B34" s="70"/>
+      <c r="C34" s="70"/>
     </row>
     <row r="35" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="38"/>
@@ -3856,20 +3859,20 @@
     </row>
     <row r="37" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="5" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
       <c r="B37" s="6"/>
       <c r="C37" s="6" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="41" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="B38" s="9"/>
       <c r="C38" s="9" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
@@ -3883,11 +3886,11 @@
       <c r="C40" s="15"/>
     </row>
     <row r="41" spans="1:3" ht="38.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="73" t="s">
-        <v>127</v>
-      </c>
-      <c r="B41" s="73"/>
-      <c r="C41" s="73"/>
+      <c r="A41" s="77" t="s">
+        <v>118</v>
+      </c>
+      <c r="B41" s="77"/>
+      <c r="C41" s="77"/>
     </row>
     <row r="42" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="38"/>
@@ -3907,20 +3910,20 @@
     </row>
     <row r="44" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="5" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="B44" s="6"/>
       <c r="C44" s="6" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="41" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="B45" s="9"/>
       <c r="C45" s="9" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
@@ -3937,19 +3940,19 @@
       <c r="A48" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B48" s="74" t="s">
+      <c r="B48" s="73" t="s">
         <v>39</v>
       </c>
-      <c r="C48" s="74"/>
+      <c r="C48" s="73"/>
     </row>
     <row r="49" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B49" s="71" t="s">
-        <v>124</v>
-      </c>
-      <c r="C49" s="71"/>
+      <c r="B49" s="75" t="s">
+        <v>115</v>
+      </c>
+      <c r="C49" s="75"/>
     </row>
     <row r="50" spans="1:3" s="61" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="59"/>
@@ -3962,11 +3965,11 @@
       <c r="C51" s="43"/>
     </row>
     <row r="52" spans="1:3" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="72" t="s">
+      <c r="A52" s="70" t="s">
         <v>23</v>
       </c>
-      <c r="B52" s="72"/>
-      <c r="C52" s="72"/>
+      <c r="B52" s="70"/>
+      <c r="C52" s="70"/>
     </row>
     <row r="53" spans="1:3" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="40"/>
@@ -3977,28 +3980,28 @@
       <c r="A54" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B54" s="70" t="s">
+      <c r="B54" s="76" t="s">
         <v>36</v>
       </c>
-      <c r="C54" s="70"/>
+      <c r="C54" s="76"/>
     </row>
     <row r="55" spans="1:3" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B55" s="71" t="s">
-        <v>128</v>
-      </c>
-      <c r="C55" s="71"/>
+      <c r="B55" s="75" t="s">
+        <v>119</v>
+      </c>
+      <c r="C55" s="75"/>
     </row>
     <row r="56" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B56" s="70" t="s">
+      <c r="B56" s="76" t="s">
         <v>36</v>
       </c>
-      <c r="C56" s="70"/>
+      <c r="C56" s="76"/>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="32"/>
@@ -4008,17 +4011,6 @@
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="19">
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="A13:C13"/>
-    <mergeCell ref="A25:C25"/>
     <mergeCell ref="A52:C52"/>
     <mergeCell ref="B54:C54"/>
     <mergeCell ref="B55:C55"/>
@@ -4027,6 +4019,17 @@
     <mergeCell ref="B48:C48"/>
     <mergeCell ref="B49:C49"/>
     <mergeCell ref="A41:C41"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="A13:C13"/>
+    <mergeCell ref="A25:C25"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B6:C6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4037,7 +4040,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7A8B418-3D2D-43BC-9E5D-E5F20215EE0A}">
   <dimension ref="A1:G57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
@@ -4050,7 +4053,7 @@
   <sheetData>
     <row r="1" spans="1:3" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="78" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
       <c r="B1" s="79"/>
       <c r="C1" s="80"/>
@@ -4064,73 +4067,73 @@
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="74">
+      <c r="B3" s="73">
         <v>6</v>
       </c>
-      <c r="C3" s="74"/>
+      <c r="C3" s="73"/>
     </row>
     <row r="4" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="77" t="s">
-        <v>130</v>
-      </c>
-      <c r="C4" s="77"/>
+      <c r="B4" s="74" t="s">
+        <v>121</v>
+      </c>
+      <c r="C4" s="74"/>
     </row>
     <row r="5" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B5" s="70" t="s">
-        <v>97</v>
-      </c>
-      <c r="C5" s="70"/>
+      <c r="B5" s="76" t="s">
+        <v>88</v>
+      </c>
+      <c r="C5" s="76"/>
     </row>
     <row r="6" spans="1:3" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="71" t="s">
-        <v>131</v>
-      </c>
-      <c r="C6" s="71"/>
+      <c r="B6" s="75" t="s">
+        <v>122</v>
+      </c>
+      <c r="C6" s="75"/>
     </row>
     <row r="7" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="70" t="s">
+      <c r="B7" s="76" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="70"/>
+      <c r="C7" s="76"/>
     </row>
     <row r="8" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="76">
+      <c r="B8" s="72">
         <v>43309</v>
       </c>
-      <c r="C8" s="76"/>
+      <c r="C8" s="72"/>
     </row>
     <row r="9" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="70" t="s">
-        <v>112</v>
-      </c>
-      <c r="C9" s="70"/>
+      <c r="B9" s="76" t="s">
+        <v>103</v>
+      </c>
+      <c r="C9" s="76"/>
     </row>
     <row r="10" spans="1:3" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="75" t="s">
-        <v>132</v>
-      </c>
-      <c r="C10" s="75"/>
+      <c r="B10" s="71" t="s">
+        <v>123</v>
+      </c>
+      <c r="C10" s="71"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="36"/>
@@ -4143,11 +4146,11 @@
       <c r="C12" s="28"/>
     </row>
     <row r="13" spans="1:3" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="72" t="s">
+      <c r="A13" s="70" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="72"/>
-      <c r="C13" s="72"/>
+      <c r="B13" s="70"/>
+      <c r="C13" s="70"/>
     </row>
     <row r="14" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="38"/>
@@ -4171,7 +4174,7 @@
       </c>
       <c r="B16" s="6"/>
       <c r="C16" s="6" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4179,7 +4182,7 @@
         <v>8</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="C17" s="8"/>
     </row>
@@ -4189,7 +4192,7 @@
       </c>
       <c r="B18" s="6"/>
       <c r="C18" s="6" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4197,7 +4200,7 @@
         <v>10</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
       <c r="C19" s="9"/>
     </row>
@@ -4207,7 +4210,7 @@
       </c>
       <c r="B20" s="6"/>
       <c r="C20" s="6" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4216,7 +4219,7 @@
       </c>
       <c r="B21" s="9"/>
       <c r="C21" s="9" t="s">
-        <v>171</v>
+        <v>156</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4225,43 +4228,43 @@
       </c>
       <c r="B22" s="6"/>
       <c r="C22" s="6" t="s">
-        <v>176</v>
+        <v>161</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="41" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="C23" s="9"/>
     </row>
     <row r="24" spans="1:3" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="B24" s="6"/>
       <c r="C24" s="6" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="41" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
       <c r="B25" s="9"/>
       <c r="C25" s="9" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="5" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="B26" s="6"/>
       <c r="C26" s="6" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -4275,11 +4278,11 @@
       <c r="C28" s="31"/>
     </row>
     <row r="29" spans="1:3" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="72" t="s">
+      <c r="A29" s="70" t="s">
         <v>19</v>
       </c>
-      <c r="B29" s="72"/>
-      <c r="C29" s="72"/>
+      <c r="B29" s="70"/>
+      <c r="C29" s="70"/>
     </row>
     <row r="30" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="38"/>
@@ -4302,7 +4305,7 @@
         <v>42</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>168</v>
+        <v>153</v>
       </c>
       <c r="C32" s="6"/>
     </row>
@@ -4311,52 +4314,52 @@
         <v>20</v>
       </c>
       <c r="B33" s="9" t="s">
-        <v>169</v>
+        <v>154</v>
       </c>
       <c r="C33" s="9"/>
     </row>
     <row r="34" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="5" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>167</v>
+        <v>152</v>
       </c>
       <c r="C34" s="6"/>
     </row>
     <row r="35" spans="1:7" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="41" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="B35" s="9" t="s">
-        <v>169</v>
+        <v>154</v>
       </c>
       <c r="C35" s="9"/>
     </row>
     <row r="36" spans="1:7" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="69" t="s">
-        <v>160</v>
+        <v>145</v>
       </c>
       <c r="B36" s="68" t="s">
-        <v>170</v>
+        <v>155</v>
       </c>
       <c r="C36" s="6"/>
     </row>
     <row r="37" spans="1:7" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="41" t="s">
-        <v>161</v>
+        <v>146</v>
       </c>
       <c r="B37" s="9" t="s">
-        <v>178</v>
+        <v>163</v>
       </c>
       <c r="C37" s="9"/>
     </row>
     <row r="38" spans="1:7" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="5" t="s">
-        <v>177</v>
+        <v>162</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>169</v>
+        <v>154</v>
       </c>
       <c r="C38" s="6"/>
       <c r="G38" s="31"/>
@@ -4372,11 +4375,11 @@
       <c r="C40" s="15"/>
     </row>
     <row r="41" spans="1:7" ht="38.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="73" t="s">
-        <v>172</v>
-      </c>
-      <c r="B41" s="73"/>
-      <c r="C41" s="73"/>
+      <c r="A41" s="77" t="s">
+        <v>157</v>
+      </c>
+      <c r="B41" s="77"/>
+      <c r="C41" s="77"/>
     </row>
     <row r="42" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="38"/>
@@ -4396,16 +4399,16 @@
     </row>
     <row r="44" spans="1:7" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="5" t="s">
-        <v>173</v>
+        <v>158</v>
       </c>
       <c r="B44" s="6"/>
       <c r="C44" s="6" t="s">
-        <v>174</v>
+        <v>159</v>
       </c>
     </row>
     <row r="45" spans="1:7" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="7" t="s">
-        <v>175</v>
+        <v>160</v>
       </c>
       <c r="B45" s="10"/>
       <c r="C45" s="10" t="s">
@@ -4426,19 +4429,19 @@
       <c r="A48" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B48" s="74" t="s">
-        <v>179</v>
-      </c>
-      <c r="C48" s="74"/>
+      <c r="B48" s="73" t="s">
+        <v>164</v>
+      </c>
+      <c r="C48" s="73"/>
     </row>
     <row r="49" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B49" s="71" t="s">
-        <v>180</v>
-      </c>
-      <c r="C49" s="71"/>
+      <c r="B49" s="75" t="s">
+        <v>165</v>
+      </c>
+      <c r="C49" s="75"/>
     </row>
     <row r="50" spans="1:3" s="61" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="59"/>
@@ -4451,11 +4454,11 @@
       <c r="C51" s="43"/>
     </row>
     <row r="52" spans="1:3" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="72" t="s">
+      <c r="A52" s="70" t="s">
         <v>23</v>
       </c>
-      <c r="B52" s="72"/>
-      <c r="C52" s="72"/>
+      <c r="B52" s="70"/>
+      <c r="C52" s="70"/>
     </row>
     <row r="53" spans="1:3" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="40"/>
@@ -4466,28 +4469,28 @@
       <c r="A54" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B54" s="70" t="s">
+      <c r="B54" s="76" t="s">
         <v>36</v>
       </c>
-      <c r="C54" s="70"/>
+      <c r="C54" s="76"/>
     </row>
     <row r="55" spans="1:3" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B55" s="71" t="s">
-        <v>181</v>
-      </c>
-      <c r="C55" s="71"/>
+      <c r="B55" s="75" t="s">
+        <v>166</v>
+      </c>
+      <c r="C55" s="75"/>
     </row>
     <row r="56" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B56" s="70" t="s">
+      <c r="B56" s="76" t="s">
         <v>36</v>
       </c>
-      <c r="C56" s="70"/>
+      <c r="C56" s="76"/>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="32"/>
@@ -4497,12 +4500,6 @@
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="18">
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B6:C6"/>
     <mergeCell ref="B56:C56"/>
     <mergeCell ref="B8:C8"/>
     <mergeCell ref="B9:C9"/>
@@ -4515,6 +4512,12 @@
     <mergeCell ref="B54:C54"/>
     <mergeCell ref="B55:C55"/>
     <mergeCell ref="A41:C41"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B6:C6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4537,7 +4540,7 @@
   <sheetData>
     <row r="1" spans="1:3" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="78" t="s">
-        <v>184</v>
+        <v>169</v>
       </c>
       <c r="B1" s="79"/>
       <c r="C1" s="80"/>
@@ -4551,73 +4554,73 @@
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="74">
+      <c r="B3" s="73">
         <v>7</v>
       </c>
-      <c r="C3" s="74"/>
+      <c r="C3" s="73"/>
     </row>
     <row r="4" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="77" t="s">
-        <v>185</v>
-      </c>
-      <c r="C4" s="77"/>
+      <c r="B4" s="74" t="s">
+        <v>170</v>
+      </c>
+      <c r="C4" s="74"/>
     </row>
     <row r="5" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B5" s="70" t="s">
+      <c r="B5" s="76" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="70"/>
+      <c r="C5" s="76"/>
     </row>
     <row r="6" spans="1:3" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="71" t="s">
-        <v>186</v>
-      </c>
-      <c r="C6" s="71"/>
+      <c r="B6" s="75" t="s">
+        <v>171</v>
+      </c>
+      <c r="C6" s="75"/>
     </row>
     <row r="7" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="70" t="s">
+      <c r="B7" s="76" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="70"/>
+      <c r="C7" s="76"/>
     </row>
     <row r="8" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="76">
+      <c r="B8" s="72">
         <v>43310</v>
       </c>
-      <c r="C8" s="76"/>
+      <c r="C8" s="72"/>
     </row>
     <row r="9" spans="1:3" ht="47.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="70" t="s">
-        <v>203</v>
-      </c>
-      <c r="C9" s="70"/>
+      <c r="B9" s="76" t="s">
+        <v>188</v>
+      </c>
+      <c r="C9" s="76"/>
     </row>
     <row r="10" spans="1:3" ht="46.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="75" t="s">
-        <v>189</v>
-      </c>
-      <c r="C10" s="75"/>
+      <c r="B10" s="71" t="s">
+        <v>174</v>
+      </c>
+      <c r="C10" s="71"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="36"/>
@@ -4630,11 +4633,11 @@
       <c r="C12" s="28"/>
     </row>
     <row r="13" spans="1:3" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="72" t="s">
+      <c r="A13" s="70" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="72"/>
-      <c r="C13" s="72"/>
+      <c r="B13" s="70"/>
+      <c r="C13" s="70"/>
     </row>
     <row r="14" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="38"/>
@@ -4658,7 +4661,7 @@
       </c>
       <c r="B16" s="6"/>
       <c r="C16" s="6" t="s">
-        <v>191</v>
+        <v>176</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4666,7 +4669,7 @@
         <v>8</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>190</v>
+        <v>175</v>
       </c>
       <c r="C17" s="8"/>
     </row>
@@ -4676,7 +4679,7 @@
       </c>
       <c r="B18" s="6"/>
       <c r="C18" s="6" t="s">
-        <v>192</v>
+        <v>177</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4685,7 +4688,7 @@
       </c>
       <c r="B19" s="9"/>
       <c r="C19" s="9" t="s">
-        <v>193</v>
+        <v>178</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4694,7 +4697,7 @@
       </c>
       <c r="B20" s="6"/>
       <c r="C20" s="6" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -4708,11 +4711,11 @@
       <c r="C22" s="31"/>
     </row>
     <row r="23" spans="1:3" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="72" t="s">
+      <c r="A23" s="70" t="s">
         <v>19</v>
       </c>
-      <c r="B23" s="72"/>
-      <c r="C23" s="72"/>
+      <c r="B23" s="70"/>
+      <c r="C23" s="70"/>
     </row>
     <row r="24" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="38"/>
@@ -4735,7 +4738,7 @@
         <v>17</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>214</v>
+        <v>199</v>
       </c>
       <c r="C26" s="6"/>
     </row>
@@ -4744,16 +4747,16 @@
         <v>20</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>195</v>
+        <v>180</v>
       </c>
       <c r="C27" s="9"/>
     </row>
     <row r="28" spans="1:3" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="5" t="s">
-        <v>194</v>
+        <v>179</v>
       </c>
       <c r="B28" s="68" t="s">
-        <v>215</v>
+        <v>200</v>
       </c>
       <c r="C28" s="6"/>
     </row>
@@ -4768,11 +4771,11 @@
       <c r="C30" s="15"/>
     </row>
     <row r="31" spans="1:3" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="72" t="s">
-        <v>196</v>
-      </c>
-      <c r="B31" s="72"/>
-      <c r="C31" s="72"/>
+      <c r="A31" s="70" t="s">
+        <v>181</v>
+      </c>
+      <c r="B31" s="70"/>
+      <c r="C31" s="70"/>
     </row>
     <row r="32" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="38"/>
@@ -4792,7 +4795,7 @@
     </row>
     <row r="34" spans="1:3" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="5" t="s">
-        <v>197</v>
+        <v>182</v>
       </c>
       <c r="B34" s="6"/>
       <c r="C34" s="6" t="s">
@@ -4801,20 +4804,20 @@
     </row>
     <row r="35" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="7" t="s">
-        <v>198</v>
+        <v>183</v>
       </c>
       <c r="B35" s="10"/>
       <c r="C35" s="9" t="s">
-        <v>200</v>
+        <v>185</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="5" t="s">
-        <v>199</v>
+        <v>184</v>
       </c>
       <c r="B36" s="6"/>
       <c r="C36" s="6" t="s">
-        <v>218</v>
+        <v>203</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
@@ -4831,19 +4834,19 @@
       <c r="A39" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B39" s="74" t="s">
-        <v>201</v>
-      </c>
-      <c r="C39" s="74"/>
+      <c r="B39" s="73" t="s">
+        <v>186</v>
+      </c>
+      <c r="C39" s="73"/>
     </row>
     <row r="40" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B40" s="71" t="s">
-        <v>202</v>
-      </c>
-      <c r="C40" s="71"/>
+      <c r="B40" s="75" t="s">
+        <v>187</v>
+      </c>
+      <c r="C40" s="75"/>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="59"/>
@@ -4856,11 +4859,11 @@
       <c r="C42" s="43"/>
     </row>
     <row r="43" spans="1:3" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="72" t="s">
+      <c r="A43" s="70" t="s">
         <v>23</v>
       </c>
-      <c r="B43" s="72"/>
-      <c r="C43" s="72"/>
+      <c r="B43" s="70"/>
+      <c r="C43" s="70"/>
     </row>
     <row r="44" spans="1:3" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="40"/>
@@ -4871,28 +4874,28 @@
       <c r="A45" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B45" s="70" t="s">
+      <c r="B45" s="76" t="s">
         <v>36</v>
       </c>
-      <c r="C45" s="70"/>
+      <c r="C45" s="76"/>
     </row>
     <row r="46" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B46" s="71" t="s">
-        <v>204</v>
-      </c>
-      <c r="C46" s="71"/>
+      <c r="B46" s="75" t="s">
+        <v>189</v>
+      </c>
+      <c r="C46" s="75"/>
     </row>
     <row r="47" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B47" s="70" t="s">
+      <c r="B47" s="76" t="s">
         <v>36</v>
       </c>
-      <c r="C47" s="70"/>
+      <c r="C47" s="76"/>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="32"/>
@@ -4902,6 +4905,12 @@
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="18">
+    <mergeCell ref="A43:C43"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="B40:C40"/>
     <mergeCell ref="A31:C31"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="B3:C3"/>
@@ -4914,12 +4923,6 @@
     <mergeCell ref="B10:C10"/>
     <mergeCell ref="A13:C13"/>
     <mergeCell ref="A23:C23"/>
-    <mergeCell ref="A43:C43"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="B46:C46"/>
-    <mergeCell ref="B47:C47"/>
-    <mergeCell ref="B39:C39"/>
-    <mergeCell ref="B40:C40"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4942,7 +4945,7 @@
   <sheetData>
     <row r="1" spans="1:3" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="78" t="s">
-        <v>205</v>
+        <v>190</v>
       </c>
       <c r="B1" s="79"/>
       <c r="C1" s="80"/>
@@ -4956,73 +4959,73 @@
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="74">
+      <c r="B3" s="73">
         <v>8</v>
       </c>
-      <c r="C3" s="74"/>
+      <c r="C3" s="73"/>
     </row>
     <row r="4" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="77" t="s">
-        <v>208</v>
-      </c>
-      <c r="C4" s="77"/>
+      <c r="B4" s="74" t="s">
+        <v>193</v>
+      </c>
+      <c r="C4" s="74"/>
     </row>
     <row r="5" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B5" s="70" t="s">
-        <v>207</v>
-      </c>
-      <c r="C5" s="70"/>
+      <c r="B5" s="76" t="s">
+        <v>192</v>
+      </c>
+      <c r="C5" s="76"/>
     </row>
     <row r="6" spans="1:3" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="71" t="s">
+      <c r="B6" s="75" t="s">
         <v>40</v>
       </c>
-      <c r="C6" s="71"/>
+      <c r="C6" s="75"/>
     </row>
     <row r="7" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="70" t="s">
+      <c r="B7" s="76" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="70"/>
+      <c r="C7" s="76"/>
     </row>
     <row r="8" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="76">
+      <c r="B8" s="72">
         <v>43310</v>
       </c>
-      <c r="C8" s="76"/>
+      <c r="C8" s="72"/>
     </row>
     <row r="9" spans="1:3" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="70" t="s">
-        <v>206</v>
-      </c>
-      <c r="C9" s="70"/>
+      <c r="B9" s="76" t="s">
+        <v>191</v>
+      </c>
+      <c r="C9" s="76"/>
     </row>
     <row r="10" spans="1:3" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="75" t="s">
-        <v>211</v>
-      </c>
-      <c r="C10" s="75"/>
+      <c r="B10" s="71" t="s">
+        <v>196</v>
+      </c>
+      <c r="C10" s="71"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="36"/>
@@ -5035,11 +5038,11 @@
       <c r="C12" s="28"/>
     </row>
     <row r="13" spans="1:3" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="72" t="s">
+      <c r="A13" s="70" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="72"/>
-      <c r="C13" s="72"/>
+      <c r="B13" s="70"/>
+      <c r="C13" s="70"/>
     </row>
     <row r="14" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="38"/>
@@ -5063,7 +5066,7 @@
       </c>
       <c r="B16" s="6"/>
       <c r="C16" s="6" t="s">
-        <v>213</v>
+        <v>198</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5071,7 +5074,7 @@
         <v>8</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>190</v>
+        <v>175</v>
       </c>
       <c r="C17" s="9"/>
     </row>
@@ -5081,7 +5084,7 @@
       </c>
       <c r="B18" s="6"/>
       <c r="C18" s="6" t="s">
-        <v>210</v>
+        <v>195</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5090,7 +5093,7 @@
       </c>
       <c r="B19" s="9"/>
       <c r="C19" s="9" t="s">
-        <v>209</v>
+        <v>194</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5099,7 +5102,7 @@
       </c>
       <c r="B20" s="6"/>
       <c r="C20" s="6" t="s">
-        <v>212</v>
+        <v>197</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -5113,11 +5116,11 @@
       <c r="C22" s="31"/>
     </row>
     <row r="23" spans="1:3" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="72" t="s">
+      <c r="A23" s="70" t="s">
         <v>19</v>
       </c>
-      <c r="B23" s="72"/>
-      <c r="C23" s="72"/>
+      <c r="B23" s="70"/>
+      <c r="C23" s="70"/>
     </row>
     <row r="24" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="38"/>
@@ -5140,7 +5143,7 @@
         <v>17</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>214</v>
+        <v>199</v>
       </c>
       <c r="C26" s="6"/>
     </row>
@@ -5149,16 +5152,16 @@
         <v>20</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>195</v>
+        <v>180</v>
       </c>
       <c r="C27" s="9"/>
     </row>
     <row r="28" spans="1:3" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="5" t="s">
-        <v>194</v>
+        <v>179</v>
       </c>
       <c r="B28" s="68" t="s">
-        <v>215</v>
+        <v>200</v>
       </c>
       <c r="C28" s="6"/>
     </row>
@@ -5173,11 +5176,11 @@
       <c r="C30" s="15"/>
     </row>
     <row r="31" spans="1:3" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="72" t="s">
-        <v>216</v>
-      </c>
-      <c r="B31" s="72"/>
-      <c r="C31" s="72"/>
+      <c r="A31" s="70" t="s">
+        <v>201</v>
+      </c>
+      <c r="B31" s="70"/>
+      <c r="C31" s="70"/>
     </row>
     <row r="32" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="38"/>
@@ -5197,7 +5200,7 @@
     </row>
     <row r="34" spans="1:3" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="5" t="s">
-        <v>197</v>
+        <v>182</v>
       </c>
       <c r="B34" s="6"/>
       <c r="C34" s="6" t="s">
@@ -5206,20 +5209,20 @@
     </row>
     <row r="35" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="7" t="s">
-        <v>198</v>
+        <v>183</v>
       </c>
       <c r="B35" s="10"/>
       <c r="C35" s="9" t="s">
-        <v>217</v>
+        <v>202</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="5" t="s">
-        <v>199</v>
+        <v>184</v>
       </c>
       <c r="B36" s="6"/>
       <c r="C36" s="6" t="s">
-        <v>218</v>
+        <v>203</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
@@ -5236,19 +5239,19 @@
       <c r="A39" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B39" s="74" t="s">
-        <v>201</v>
-      </c>
-      <c r="C39" s="74"/>
+      <c r="B39" s="73" t="s">
+        <v>186</v>
+      </c>
+      <c r="C39" s="73"/>
     </row>
     <row r="40" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B40" s="71" t="s">
-        <v>219</v>
-      </c>
-      <c r="C40" s="71"/>
+      <c r="B40" s="75" t="s">
+        <v>204</v>
+      </c>
+      <c r="C40" s="75"/>
     </row>
     <row r="41" spans="1:3" s="61" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="59"/>
@@ -5261,11 +5264,11 @@
       <c r="C42" s="43"/>
     </row>
     <row r="43" spans="1:3" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="72" t="s">
+      <c r="A43" s="70" t="s">
         <v>23</v>
       </c>
-      <c r="B43" s="72"/>
-      <c r="C43" s="72"/>
+      <c r="B43" s="70"/>
+      <c r="C43" s="70"/>
     </row>
     <row r="44" spans="1:3" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="40"/>
@@ -5276,28 +5279,28 @@
       <c r="A45" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B45" s="70" t="s">
+      <c r="B45" s="76" t="s">
         <v>36</v>
       </c>
-      <c r="C45" s="70"/>
+      <c r="C45" s="76"/>
     </row>
     <row r="46" spans="1:3" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B46" s="71" t="s">
+      <c r="B46" s="75" t="s">
         <v>41</v>
       </c>
-      <c r="C46" s="71"/>
+      <c r="C46" s="75"/>
     </row>
     <row r="47" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B47" s="70" t="s">
+      <c r="B47" s="76" t="s">
         <v>36</v>
       </c>
-      <c r="C47" s="70"/>
+      <c r="C47" s="76"/>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="32"/>
@@ -5307,6 +5310,12 @@
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="18">
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B6:C6"/>
     <mergeCell ref="B47:C47"/>
     <mergeCell ref="A43:C43"/>
     <mergeCell ref="B45:C45"/>
@@ -5319,12 +5328,6 @@
     <mergeCell ref="A31:C31"/>
     <mergeCell ref="B39:C39"/>
     <mergeCell ref="B40:C40"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B6:C6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>